<commit_message>
updates for stage 3
</commit_message>
<xml_diff>
--- a/Quroum_Round_USA/Stage 3/StateToState.xlsx
+++ b/Quroum_Round_USA/Stage 3/StateToState.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\A_Quorum_Journey\Quroum_Round_USA\Stage 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D66BE44E-D6F5-430E-8C83-B4BE262C72F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8CB78D-320D-4BC3-A865-2DC883FC9BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37620" yWindow="-2565" windowWidth="34290" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All States" sheetId="1" r:id="rId1"/>
@@ -2463,7 +2463,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>